<commit_message>
testdata: update sample Excel for chunker preview validation
</commit_message>
<xml_diff>
--- a/testdata/public/test_excel_table_and_description.xlsx
+++ b/testdata/public/test_excel_table_and_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AtsushiSuzuki\docs\rust\hybrid-search-rs-4\testdata\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B81746-40C4-443F-9D64-807A9FF00204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4B959E-5224-4999-8EAF-FE500E96CEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26730" yWindow="1090" windowWidth="22220" windowHeight="17530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26960" yWindow="1320" windowWidth="22220" windowHeight="17530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="販売データ" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>商品名</t>
   </si>
@@ -148,6 +148,55 @@
     </rPh>
     <rPh sb="19" eb="20">
       <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この行の前に、1行空白があります。</t>
+    <rPh sb="2" eb="3">
+      <t>ギョウ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>ギョウクウハク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>空白行がある場合</t>
+    <rPh sb="0" eb="2">
+      <t>クウハク</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ギョウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>空白列がある場合</t>
+    <rPh sb="0" eb="3">
+      <t>クウハクレツ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このセルの前に、1列空白のセルがあります。</t>
+    <rPh sb="5" eb="6">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>レツ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>クウハク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -623,7 +672,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -706,6 +755,22 @@
       </c>
       <c r="D8" s="2"/>
     </row>
+    <row r="10" spans="2:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C8:D8"/>

</xml_diff>